<commit_message>
update estimates of maximum offsets for Scenario 3
</commit_message>
<xml_diff>
--- a/Teleconnections/Offsets.xlsx
+++ b/Teleconnections/Offsets.xlsx
@@ -185,9 +185,6 @@
     <t>http://arc-lter.ecosystems.mbl.edu/toolik-main</t>
   </si>
   <si>
-    <t>Max ElNino year</t>
-  </si>
-  <si>
     <t>Scenario2: offset for 2013 based on linear fits of ElNino years vs. Neutral years</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>has inflows/outflows but don't have year's worth of flows</t>
+  </si>
+  <si>
+    <t>Max offset year</t>
   </si>
 </sst>
 </file>
@@ -598,21 +598,21 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="6" max="6" width="9.875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="40.25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15" style="1" customWidth="1"/>
     <col min="11" max="12" width="15.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.5" style="2" bestFit="1" customWidth="1"/>
@@ -643,13 +643,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>7</v>
@@ -696,7 +696,7 @@
         <v>0.42339700000000002</v>
       </c>
       <c r="I2" s="2">
-        <v>1.271647</v>
+        <v>1.27</v>
       </c>
       <c r="J2" s="1">
         <v>1982</v>
@@ -746,7 +746,7 @@
         <v>0.88025359999999997</v>
       </c>
       <c r="I3" s="2">
-        <v>2.813367</v>
+        <v>2.81</v>
       </c>
       <c r="J3" s="1">
         <v>1998</v>
@@ -796,7 +796,7 @@
         <v>0.22417300000000001</v>
       </c>
       <c r="I4" s="2">
-        <v>1.2880549999999999</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="J4" s="1">
         <v>1991</v>
@@ -846,7 +846,7 @@
         <v>0.89095250000000004</v>
       </c>
       <c r="I5" s="2">
-        <v>1.9135530000000001</v>
+        <v>1.91</v>
       </c>
       <c r="J5" s="1">
         <v>1998</v>
@@ -896,7 +896,7 @@
         <v>0.1329429</v>
       </c>
       <c r="I6" s="2">
-        <v>1.5547340000000001</v>
+        <v>1.55</v>
       </c>
       <c r="J6" s="1">
         <v>1998</v>
@@ -943,7 +943,7 @@
         <v>-89.704767000000004</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -983,7 +983,7 @@
         <v>-99.117631000000003</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
@@ -1014,7 +1014,7 @@
         <v>1.636306</v>
       </c>
       <c r="I9" s="2">
-        <v>3.7864749999999998</v>
+        <v>3.79</v>
       </c>
       <c r="J9" s="1">
         <v>1987</v>
@@ -1064,7 +1064,7 @@
         <v>0.42339700000000002</v>
       </c>
       <c r="I10" s="2">
-        <v>1.271647</v>
+        <v>1.27</v>
       </c>
       <c r="J10" s="1">
         <v>1982</v>
@@ -1111,7 +1111,7 @@
         <v>-149.61051</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I11" s="15"/>
       <c r="J11" s="15"/>

</xml_diff>

<commit_message>
update testing script to include plotting for assessments
</commit_message>
<xml_diff>
--- a/Teleconnections/Offsets.xlsx
+++ b/Teleconnections/Offsets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
   <si>
     <t>Lake Name</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Scenario3: offset based on highest-offset year mean Air Temp vs. that year's estimated Air Temp based on Neutral years</t>
-  </si>
-  <si>
-    <t>no NLDAS data</t>
   </si>
   <si>
     <t>has inflows/outflows but don't have year's worth of flows</t>
@@ -287,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -314,6 +311,8 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -598,7 +597,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -620,7 +619,7 @@
     <col min="16" max="16" width="66.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="11" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="11" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -649,7 +648,7 @@
         <v>54</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>7</v>
@@ -943,7 +942,7 @@
         <v>-89.704767000000004</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15"/>
@@ -983,7 +982,7 @@
         <v>-99.117631000000003</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
@@ -1110,11 +1109,15 @@
       <c r="G11" s="8">
         <v>-149.61051</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="H11" s="16">
+        <v>1.189862</v>
+      </c>
+      <c r="I11" s="16">
+        <v>6.3348899999999997</v>
+      </c>
+      <c r="J11" s="17">
+        <v>1993</v>
+      </c>
       <c r="K11" s="8" t="s">
         <v>50</v>
       </c>
@@ -1138,8 +1141,7 @@
       <c r="P17" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="H11:J11"/>
+  <mergeCells count="2">
     <mergeCell ref="H7:J7"/>
     <mergeCell ref="H8:J8"/>
   </mergeCells>

</xml_diff>